<commit_message>
Notas 13 Oct 2022
</commit_message>
<xml_diff>
--- a/Notas UCSM 2022B.xlsx
+++ b/Notas UCSM 2022B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlocorrales/Documents/UCSM/UCSMn/Notas UCSM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F170FB07-565B-B746-BC12-5402223F2F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6299A8D3-8C6B-9A4F-BCD8-B9B7853A7F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="15000" activeTab="2" xr2:uid="{FDD2B5AD-8C9F-C940-A737-C661D3C2DF6A}"/>
+    <workbookView xWindow="19040" yWindow="17820" windowWidth="52040" windowHeight="22740" activeTab="2" xr2:uid="{FDD2B5AD-8C9F-C940-A737-C661D3C2DF6A}"/>
   </bookViews>
   <sheets>
     <sheet name="EDis1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="669">
   <si>
     <t>FLOREZ CRUZ, GONZALO GILMAR</t>
   </si>
@@ -2047,6 +2047,9 @@
   </si>
   <si>
     <t>Scotiabank</t>
+  </si>
+  <si>
+    <t>Complejdad</t>
   </si>
 </sst>
 </file>
@@ -5081,8 +5084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED02CACE-6B48-5243-AB86-D6DEC2B10933}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5095,6 +5098,7 @@
     <col min="13" max="13" width="7.83203125" style="34" customWidth="1"/>
     <col min="14" max="14" width="4.5" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" customWidth="1"/>
     <col min="19" max="19" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5133,7 +5137,9 @@
       <c r="O2" s="6" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>668</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="S2" t="s">
         <v>154</v>
@@ -5335,7 +5341,9 @@
       <c r="O6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="S6" t="s">
         <v>200</v>
@@ -5393,7 +5401,9 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1">
+        <v>3</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="S7" t="s">
         <v>208</v>
@@ -5503,7 +5513,9 @@
         <v>1</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
       <c r="Q9" s="1"/>
       <c r="S9" t="s">
         <v>227</v>
@@ -5617,7 +5629,9 @@
       <c r="O11" s="1">
         <v>1</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
       <c r="Q11" s="1"/>
       <c r="S11" t="s">
         <v>234</v>
@@ -5759,7 +5773,9 @@
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1">
+        <v>1</v>
+      </c>
       <c r="Q14" s="1"/>
       <c r="S14" t="s">
         <v>276</v>
@@ -5825,7 +5841,9 @@
       <c r="O15" s="1">
         <v>1</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="S15" t="s">
         <v>309</v>
@@ -6185,7 +6203,9 @@
       <c r="O22" s="1">
         <v>1</v>
       </c>
-      <c r="P22" s="1"/>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="S22" t="s">
         <v>376</v>
@@ -6249,7 +6269,9 @@
       <c r="O23" s="1">
         <v>2</v>
       </c>
-      <c r="P23" s="1"/>
+      <c r="P23" s="1">
+        <v>2</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="S23" t="s">
         <v>394</v>

</xml_diff>